<commit_message>
Feat + Docs update: implementación final de menu multicajón y navegación por ID. Formateo de datos en planilla QA
</commit_message>
<xml_diff>
--- a/docs/qa_testing/planilla_casos_prueba.xlsx
+++ b/docs/qa_testing/planilla_casos_prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\NetBeansProjects\StockFreezer\docs\qa_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16882ED-1EC3-48D7-A0C7-C909117C66AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B814B06D-5B49-40C8-900F-E1D87BAFA0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Comentarios</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -307,6 +310,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -319,7 +325,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,108 +664,112 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="7">
         <v>46035</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="7"/>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="2:13" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="7">
         <v>46037</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="7"/>
+      <c r="M4" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="7">
         <v>46037</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="7">
         <v>46037</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="4" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Docs: registro de prueba exitosa CP-004 para navegación multicajón
</commit_message>
<xml_diff>
--- a/docs/qa_testing/planilla_casos_prueba.xlsx
+++ b/docs/qa_testing/planilla_casos_prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\NetBeansProjects\StockFreezer\docs\qa_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B814B06D-5B49-40C8-900F-E1D87BAFA0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3D6A17-7A1E-4779-9B97-061A0E870FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -209,12 +209,45 @@
   <si>
     <t>/</t>
   </si>
+  <si>
+    <t>CP-004</t>
+  </si>
+  <si>
+    <t>Navegación y Consistencia Multicajón</t>
+  </si>
+  <si>
+    <t>Verificar que al cambiar de cajón el mapa se adapte al tamaño real (3x4 vs 3x2) y los productos no se mezclen.</t>
+  </si>
+  <si>
+    <t>Base de datos con carga inicial (12 cajones creados).</t>
+  </si>
+  <si>
+    <t>1. Iniciar menú y elegir Cajón 12 (IDS).</t>
+  </si>
+  <si>
+    <t>2. Ver Mapa (Validar tamaño 3x2).</t>
+  </si>
+  <si>
+    <t>3. Volver y elegir Cajón 1 (IDB).</t>
+  </si>
+  <si>
+    <t>4. Ver Mapa (Validar tamaño 3x4 y que no tenga datos del cajón 12).</t>
+  </si>
+  <si>
+    <t>Cajón 12 muestra grilla chica (2 columnas). Cajón 1 muestra grilla grande (4 columnas). Los inventarios son independientes.</t>
+  </si>
+  <si>
+    <t>El sistema renderiza correctamente las matrices según el tipo de cajón. El ID 12 se identifica correctamente como "IDS-6".</t>
+  </si>
+  <si>
+    <t>Se verificó en logs que el ID 12 corresponde lógicamente al rótulo IDS-6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +299,12 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -302,16 +341,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -319,8 +358,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -605,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M5"/>
+  <dimension ref="B2:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C3" sqref="C3:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,40 +671,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -667,20 +712,20 @@
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="5" t="s">
@@ -689,13 +734,13 @@
       <c r="J3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>46035</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -703,20 +748,20 @@
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -725,13 +770,13 @@
       <c r="J4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>46037</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -739,22 +784,22 @@
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -763,17 +808,135 @@
       <c r="J5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <v>46037</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <v>46037</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="6" spans="2:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="9">
+        <v>46038</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="2:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="2:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="K6:K9"/>
+    <mergeCell ref="L6:L9"/>
+    <mergeCell ref="M6:M9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+  </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Docs: registro de falla en CP-005 con evidencia (Bug UI faltante)
</commit_message>
<xml_diff>
--- a/docs/qa_testing/planilla_casos_prueba.xlsx
+++ b/docs/qa_testing/planilla_casos_prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\NetBeansProjects\StockFreezer\docs\qa_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3D6A17-7A1E-4779-9B97-061A0E870FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B4461F-261C-4581-B873-419120EA1BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -241,6 +241,54 @@
   </si>
   <si>
     <t>Se verificó en logs que el ID 12 corresponde lógicamente al rótulo IDS-6</t>
+  </si>
+  <si>
+    <t>CP-005</t>
+  </si>
+  <si>
+    <t>Retiro de Producto (Manual)</t>
+  </si>
+  <si>
+    <t>Validar que se pueda eliminar un producto existente indicando coordenadas.</t>
+  </si>
+  <si>
+    <t>1. Ingresar al Cajón con productos.</t>
+  </si>
+  <si>
+    <t>2. Seleccionar opción de retiro.</t>
+  </si>
+  <si>
+    <t>3. Ingresar coordenadas.</t>
+  </si>
+  <si>
+    <t>4. Verificar mapa vacío.</t>
+  </si>
+  <si>
+    <t>El menú muestra la opción de retiro, el sistema borra el dato y libera el espacio visual.</t>
+  </si>
+  <si>
+    <t>Evidencia</t>
+  </si>
+  <si>
+    <r>
+      <t>FALLO BLOQUEANTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> El menú no muestra la opción "3. Retirar Producto". El usuario no sabe qué tecla tocar.</t>
+    </r>
+  </si>
+  <si>
+    <t>Existir al menos 1 producto en el cajón seleccionado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALLÓ  </t>
   </si>
 </sst>
 </file>
@@ -341,15 +389,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -364,10 +409,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -650,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M15"/>
+  <dimension ref="B2:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:M9"/>
+    <sheetView tabSelected="1" topLeftCell="F5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,11 +711,11 @@
     <col min="8" max="8" width="31.140625" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
     <col min="10" max="11" width="31.42578125" customWidth="1"/>
-    <col min="12" max="12" width="28" customWidth="1"/>
-    <col min="13" max="13" width="24.42578125" customWidth="1"/>
+    <col min="12" max="13" width="28" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -701,125 +746,131 @@
       <c r="K2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>46035</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>46037</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>46037</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>46037</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="5"/>
+      <c r="N5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -831,7 +882,7 @@
       <c r="E6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -840,101 +891,196 @@
       <c r="H6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="7">
         <v>46038</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="6"/>
+      <c r="N6" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
+    <row r="7" spans="2:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>44</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="2:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" spans="2:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="2:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="2:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="7">
+        <v>46039</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F15" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="K6:K9"/>
-    <mergeCell ref="L6:L9"/>
+  <mergeCells count="24">
+    <mergeCell ref="N10:N13"/>
     <mergeCell ref="M6:M9"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="K10:K13"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="M10:M13"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H10:H13"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="K6:K9"/>
+    <mergeCell ref="L6:L9"/>
+    <mergeCell ref="N6:N9"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix: habilito opción visual de borrar producto en Menú y actualizado QA a exitoso (PASÓ).
</commit_message>
<xml_diff>
--- a/docs/qa_testing/planilla_casos_prueba.xlsx
+++ b/docs/qa_testing/planilla_casos_prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\NetBeansProjects\StockFreezer\docs\qa_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B4461F-261C-4581-B873-419120EA1BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2109CCAA-7B7F-4C76-A228-20C1A2BE43DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -288,14 +288,17 @@
     <t>Existir al menos 1 producto en el cajón seleccionado.</t>
   </si>
   <si>
-    <t xml:space="preserve">FALLÓ  </t>
+    <t>https://github.com/Goriguen/StockFreezer/blob/10f2d977b450b81e77b3299950c65c4f9036fc87/docs/qa_testing/evidencia_screenshots/bug_cp005_menu_codigo.jpg</t>
+  </si>
+  <si>
+    <t>El sistema eliminó perfectamente el producto en las coordenadas indicadas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +356,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -386,10 +397,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -415,8 +427,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -697,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:I13"/>
+    <sheetView tabSelected="1" topLeftCell="G6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +919,9 @@
       <c r="L6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="6"/>
+      <c r="M6" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="N6" s="8" t="s">
         <v>49</v>
       </c>
@@ -985,17 +1003,19 @@
         <v>27</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="K10" s="7">
         <v>46039</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M10" s="6"/>
+      <c r="L10" s="7">
+        <v>46039</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="N10" s="8" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -1011,8 +1031,8 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="7"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
     <row r="12" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1028,8 +1048,8 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
     <row r="13" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1045,8 +1065,8 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8"/>
       <c r="N13" s="8"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
@@ -1083,6 +1103,9 @@
     <mergeCell ref="N6:N9"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="M6" r:id="rId1" xr:uid="{8CE55CA9-7E17-47E1-B6EB-4829C3BD3D9E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>